<commit_message>
improving plotting tools (HOURLY BALANCE)
</commit_message>
<xml_diff>
--- a/base/auxils/plotting_tool/input/manual_colors_input.xlsx
+++ b/base/auxils/plotting_tool/input/manual_colors_input.xlsx
@@ -1,27 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Balmorel_git\base\auxils\plotting_tool\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Balmorel\Balmorel_review\base\auxils\plotting_tool\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B05158-C1A8-4E8D-A35F-AD7BA82548F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="2090" activeTab="1"/>
+    <workbookView xWindow="9030" yWindow="1965" windowWidth="18000" windowHeight="9360" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Production" sheetId="1" r:id="rId1"/>
-    <sheet name="Demand" sheetId="2" r:id="rId2"/>
-    <sheet name="Price" sheetId="3" r:id="rId3"/>
+    <sheet name="Electricity_Production" sheetId="1" r:id="rId1"/>
+    <sheet name="Electricity_Demand" sheetId="2" r:id="rId2"/>
+    <sheet name="Electricity_Price" sheetId="3" r:id="rId3"/>
+    <sheet name="Heat_Production" sheetId="4" r:id="rId4"/>
+    <sheet name="Heat_Demand" sheetId="5" r:id="rId5"/>
+    <sheet name="Heat_Price" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>Value</t>
   </si>
@@ -44,70 +48,91 @@
     <t>red</t>
   </si>
   <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>WIND</t>
+  </si>
+  <si>
+    <t>dark blue</t>
+  </si>
+  <si>
+    <t>DEMAND_P2H</t>
+  </si>
+  <si>
+    <t>DEMAND_EXO</t>
+  </si>
+  <si>
+    <t>dark grey</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>DEMAND_LOSS</t>
+  </si>
+  <si>
+    <t>DEMAND_EV</t>
+  </si>
+  <si>
+    <t>DEMAND_CCS</t>
+  </si>
+  <si>
+    <t>DEMAND_P2G</t>
+  </si>
+  <si>
+    <t>pink</t>
+  </si>
+  <si>
+    <t>THERMAL</t>
+  </si>
+  <si>
+    <t>HYDRO</t>
+  </si>
+  <si>
+    <t>FUELCELL</t>
+  </si>
+  <si>
+    <t>DEMAND_ELSTO</t>
+  </si>
+  <si>
+    <t>SOLARPV</t>
+  </si>
+  <si>
+    <t>ELSTO</t>
+  </si>
+  <si>
+    <t>BOILERS</t>
+  </si>
+  <si>
     <t>CHP</t>
   </si>
   <si>
-    <t>green</t>
-  </si>
-  <si>
-    <t>SOLAR-PV</t>
-  </si>
-  <si>
-    <t>yellow</t>
-  </si>
-  <si>
-    <t>orange</t>
-  </si>
-  <si>
-    <t>HYDRO-RUN-OF-RIVER</t>
-  </si>
-  <si>
-    <t>CONDENSING</t>
-  </si>
-  <si>
-    <t>EL-STO</t>
-  </si>
-  <si>
-    <t>WIND</t>
-  </si>
-  <si>
-    <t>dark blue</t>
-  </si>
-  <si>
-    <t>HYDRO-RESERVOIRS</t>
-  </si>
-  <si>
-    <t>DEMAND_P2H</t>
-  </si>
-  <si>
-    <t>DEMAND_EXO</t>
-  </si>
-  <si>
-    <t>DEMAND_DISTLOSSES</t>
-  </si>
-  <si>
-    <t>DEMAND_OTHERTRANS</t>
-  </si>
-  <si>
-    <t>DEMAND_ev</t>
-  </si>
-  <si>
-    <t>dark grey</t>
-  </si>
-  <si>
-    <t>DEMAND_STO</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Black</t>
+    <t>SOLARHEATING</t>
+  </si>
+  <si>
+    <t>HEATSTO</t>
+  </si>
+  <si>
+    <t>P2H</t>
+  </si>
+  <si>
+    <t>DEMAND_HEATSTO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -907,19 +932,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B8"/>
+      <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -927,60 +952,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -989,19 +1006,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1009,52 +1026,60 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
         <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1063,16 +1088,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1080,12 +1105,172 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F88F20-02F8-4F89-B68B-18B6C7BB7335}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9000F14-F470-4C40-96B4-1C4C6948932A}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD847461-A784-4C66-BE6D-F851CE22E3CB}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>